<commit_message>
Amazon (in Trulia module), Pandora (in Verizon module), add'l Ebay pages added
</commit_message>
<xml_diff>
--- a/com.ebay/src/test/resources/test_data/EbayTestData.xlsx
+++ b/com.ebay/src/test/resources/test_data/EbayTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sami\IdeaProjects\WDE_Spring2021_SeleniumFramework\com.ebay\src\test\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980E26F7-A8EC-4C75-9AC3-3B53F92F25D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3499F813-8B92-4BDD-81CD-07BAB8B7F991}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1101C68C-BE57-4DF8-9522-5FE4B6B1B877}"/>
   </bookViews>
@@ -141,7 +141,7 @@
     <t>Everything Else</t>
   </si>
   <si>
-    <t>All Categoriess</t>
+    <t>All Categories</t>
   </si>
 </sst>
 </file>
@@ -496,7 +496,7 @@
   <dimension ref="A2:A37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>